<commit_message>
Successful Setup with LCD Display
</commit_message>
<xml_diff>
--- a/SPIRegisterSettings.xlsx
+++ b/SPIRegisterSettings.xlsx
@@ -793,10 +793,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E36"/>
+  <dimension ref="A1:O37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E36"/>
+      <selection activeCell="K2" sqref="K2:K37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -808,7 +808,7 @@
     <col min="8" max="8" width="17.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>144</v>
       </c>
@@ -825,7 +825,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -842,8 +842,12 @@
         <f>"writeSPI1("&amp;C2&amp;");writeSPI1("&amp;A2&amp;");"</f>
         <v>writeSPI1(0x0B);writeSPI1(SMARTRF_SETTING_FSCTRL1);</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="K2" t="str">
+        <f>IF(ISEVEN(ROW($K2)),"writeSPI1("&amp;$C2&amp;");","writeSPI1("&amp;$A1&amp;");")</f>
+        <v>writeSPI1(0x0B);</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -860,8 +864,16 @@
         <f t="shared" ref="E3:E36" si="0">"writeSPI1("&amp;C3&amp;");writeSPI1("&amp;A3&amp;");"</f>
         <v>writeSPI1(0x0C);writeSPI1(SMARTRF_SETTING_FSCTRL0);</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="K3" t="str">
+        <f t="shared" ref="K3:K38" si="1">IF(ISEVEN(ROW(K3)),"writeSPI1("&amp;C3&amp;");","writeSPI1("&amp;A2&amp;");")</f>
+        <v>writeSPI1(SMARTRF_SETTING_FSCTRL1);</v>
+      </c>
+      <c r="O3" t="str">
+        <f t="shared" ref="O3:O35" si="2">IF(ISODD(ROW($K3)),"writeSPI1("&amp;$C3&amp;");","writeSPI1("&amp;$A2&amp;");")</f>
+        <v>writeSPI1(0x0C);</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -878,8 +890,16 @@
         <f t="shared" si="0"/>
         <v>writeSPI1(0x0D);writeSPI1(SMARTRF_SETTING_FREQ2);</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="K4" t="str">
+        <f t="shared" si="1"/>
+        <v>writeSPI1(0x0D);</v>
+      </c>
+      <c r="O4" t="str">
+        <f t="shared" si="2"/>
+        <v>writeSPI1(SMARTRF_SETTING_FSCTRL0);</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -896,8 +916,16 @@
         <f t="shared" si="0"/>
         <v>writeSPI1(0x0E);writeSPI1(SMARTRF_SETTING_FREQ1);</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="K5" t="str">
+        <f t="shared" si="1"/>
+        <v>writeSPI1(SMARTRF_SETTING_FREQ2);</v>
+      </c>
+      <c r="O5" t="str">
+        <f t="shared" si="2"/>
+        <v>writeSPI1(0x0E);</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -914,8 +942,16 @@
         <f t="shared" si="0"/>
         <v>writeSPI1(0x0F);writeSPI1(SMARTRF_SETTING_FREQ0);</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="K6" t="str">
+        <f t="shared" si="1"/>
+        <v>writeSPI1(0x0F);</v>
+      </c>
+      <c r="O6" t="str">
+        <f t="shared" si="2"/>
+        <v>writeSPI1(SMARTRF_SETTING_FREQ1);</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -932,8 +968,16 @@
         <f t="shared" si="0"/>
         <v>writeSPI1(0x10);writeSPI1(SMARTRF_SETTING_MDMCFG4);</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="K7" t="str">
+        <f t="shared" si="1"/>
+        <v>writeSPI1(SMARTRF_SETTING_FREQ0);</v>
+      </c>
+      <c r="O7" t="str">
+        <f t="shared" si="2"/>
+        <v>writeSPI1(0x10);</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -950,8 +994,16 @@
         <f t="shared" si="0"/>
         <v>writeSPI1(0x11);writeSPI1(SMARTRF_SETTING_MDMCFG3);</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="K8" t="str">
+        <f t="shared" si="1"/>
+        <v>writeSPI1(0x11);</v>
+      </c>
+      <c r="O8" t="str">
+        <f t="shared" si="2"/>
+        <v>writeSPI1(SMARTRF_SETTING_MDMCFG4);</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -968,8 +1020,16 @@
         <f t="shared" si="0"/>
         <v>writeSPI1(0x12);writeSPI1(SMARTRF_SETTING_MDMCFG2);</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="K9" t="str">
+        <f t="shared" si="1"/>
+        <v>writeSPI1(SMARTRF_SETTING_MDMCFG3);</v>
+      </c>
+      <c r="O9" t="str">
+        <f t="shared" si="2"/>
+        <v>writeSPI1(0x12);</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -986,8 +1046,16 @@
         <f t="shared" si="0"/>
         <v>writeSPI1(0x13);writeSPI1(SMARTRF_SETTING_MDMCFG1);</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="K10" t="str">
+        <f t="shared" si="1"/>
+        <v>writeSPI1(0x13);</v>
+      </c>
+      <c r="O10" t="str">
+        <f t="shared" si="2"/>
+        <v>writeSPI1(SMARTRF_SETTING_MDMCFG2);</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -1004,8 +1072,16 @@
         <f t="shared" si="0"/>
         <v>writeSPI1(0x14);writeSPI1(SMARTRF_SETTING_MDMCFG0);</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="K11" t="str">
+        <f t="shared" si="1"/>
+        <v>writeSPI1(SMARTRF_SETTING_MDMCFG1);</v>
+      </c>
+      <c r="O11" t="str">
+        <f t="shared" si="2"/>
+        <v>writeSPI1(0x14);</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>19</v>
       </c>
@@ -1022,8 +1098,16 @@
         <f t="shared" si="0"/>
         <v>writeSPI1(0x0A);writeSPI1(SMARTRF_SETTING_CHANNR);</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="K12" t="str">
+        <f t="shared" si="1"/>
+        <v>writeSPI1(0x0A);</v>
+      </c>
+      <c r="O12" t="str">
+        <f t="shared" si="2"/>
+        <v>writeSPI1(SMARTRF_SETTING_MDMCFG0);</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>20</v>
       </c>
@@ -1040,8 +1124,16 @@
         <f t="shared" si="0"/>
         <v>writeSPI1(0x15);writeSPI1(SMARTRF_SETTING_DEVIATN);</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="K13" t="str">
+        <f t="shared" si="1"/>
+        <v>writeSPI1(SMARTRF_SETTING_CHANNR);</v>
+      </c>
+      <c r="O13" t="str">
+        <f t="shared" si="2"/>
+        <v>writeSPI1(0x15);</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>22</v>
       </c>
@@ -1058,8 +1150,16 @@
         <f t="shared" si="0"/>
         <v>writeSPI1(0x21);writeSPI1(SMARTRF_SETTING_FREND1);</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="K14" t="str">
+        <f t="shared" si="1"/>
+        <v>writeSPI1(0x21);</v>
+      </c>
+      <c r="O14" t="str">
+        <f t="shared" si="2"/>
+        <v>writeSPI1(SMARTRF_SETTING_DEVIATN);</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>24</v>
       </c>
@@ -1076,8 +1176,16 @@
         <f t="shared" si="0"/>
         <v>writeSPI1(0x22);writeSPI1(SMARTRF_SETTING_FREND0);</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="K15" t="str">
+        <f t="shared" si="1"/>
+        <v>writeSPI1(SMARTRF_SETTING_FREND1);</v>
+      </c>
+      <c r="O15" t="str">
+        <f t="shared" si="2"/>
+        <v>writeSPI1(0x22);</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>26</v>
       </c>
@@ -1094,8 +1202,16 @@
         <f t="shared" si="0"/>
         <v>writeSPI1(0x18);writeSPI1(SMARTRF_SETTING_MCSM0);</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="K16" t="str">
+        <f t="shared" si="1"/>
+        <v>writeSPI1(0x18);</v>
+      </c>
+      <c r="O16" t="str">
+        <f t="shared" si="2"/>
+        <v>writeSPI1(SMARTRF_SETTING_FREND0);</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>28</v>
       </c>
@@ -1112,8 +1228,16 @@
         <f t="shared" si="0"/>
         <v>writeSPI1(0x19);writeSPI1(SMARTRF_SETTING_FOCCFG);</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="K17" t="str">
+        <f t="shared" si="1"/>
+        <v>writeSPI1(SMARTRF_SETTING_MCSM0);</v>
+      </c>
+      <c r="O17" t="str">
+        <f t="shared" si="2"/>
+        <v>writeSPI1(0x19);</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>30</v>
       </c>
@@ -1130,8 +1254,16 @@
         <f t="shared" si="0"/>
         <v>writeSPI1(0x1A);writeSPI1(SMARTRF_SETTING_BSCFG);</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="K18" t="str">
+        <f t="shared" si="1"/>
+        <v>writeSPI1(0x1A);</v>
+      </c>
+      <c r="O18" t="str">
+        <f t="shared" si="2"/>
+        <v>writeSPI1(SMARTRF_SETTING_FOCCFG);</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>32</v>
       </c>
@@ -1148,8 +1280,16 @@
         <f t="shared" si="0"/>
         <v>writeSPI1(0x1B);writeSPI1(SMARTRF_SETTING_AGCCTRL2);</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="K19" t="str">
+        <f t="shared" si="1"/>
+        <v>writeSPI1(SMARTRF_SETTING_BSCFG);</v>
+      </c>
+      <c r="O19" t="str">
+        <f t="shared" si="2"/>
+        <v>writeSPI1(0x1B);</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>34</v>
       </c>
@@ -1166,8 +1306,16 @@
         <f t="shared" si="0"/>
         <v>writeSPI1(0x1C);writeSPI1(SMARTRF_SETTING_AGCCTRL1);</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="K20" t="str">
+        <f t="shared" si="1"/>
+        <v>writeSPI1(0x1C);</v>
+      </c>
+      <c r="O20" t="str">
+        <f t="shared" si="2"/>
+        <v>writeSPI1(SMARTRF_SETTING_AGCCTRL2);</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>35</v>
       </c>
@@ -1184,8 +1332,16 @@
         <f t="shared" si="0"/>
         <v>writeSPI1(0x1D);writeSPI1(SMARTRF_SETTING_AGCCTRL0);</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="K21" t="str">
+        <f t="shared" si="1"/>
+        <v>writeSPI1(SMARTRF_SETTING_AGCCTRL1);</v>
+      </c>
+      <c r="O21" t="str">
+        <f t="shared" si="2"/>
+        <v>writeSPI1(0x1D);</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>37</v>
       </c>
@@ -1202,8 +1358,16 @@
         <f t="shared" si="0"/>
         <v>writeSPI1(0x23);writeSPI1(SMARTRF_SETTING_FSCAL3);</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="K22" t="str">
+        <f t="shared" si="1"/>
+        <v>writeSPI1(0x23);</v>
+      </c>
+      <c r="O22" t="str">
+        <f t="shared" si="2"/>
+        <v>writeSPI1(SMARTRF_SETTING_AGCCTRL0);</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>39</v>
       </c>
@@ -1220,8 +1384,16 @@
         <f t="shared" si="0"/>
         <v>writeSPI1(0x24);writeSPI1(SMARTRF_SETTING_FSCAL2);</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="K23" t="str">
+        <f t="shared" si="1"/>
+        <v>writeSPI1(SMARTRF_SETTING_FSCAL3);</v>
+      </c>
+      <c r="O23" t="str">
+        <f t="shared" si="2"/>
+        <v>writeSPI1(0x24);</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>41</v>
       </c>
@@ -1238,8 +1410,16 @@
         <f t="shared" si="0"/>
         <v>writeSPI1(0x25);writeSPI1(SMARTRF_SETTING_FSCAL1);</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="K24" t="str">
+        <f t="shared" si="1"/>
+        <v>writeSPI1(0x25);</v>
+      </c>
+      <c r="O24" t="str">
+        <f t="shared" si="2"/>
+        <v>writeSPI1(SMARTRF_SETTING_FSCAL2);</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>42</v>
       </c>
@@ -1256,8 +1436,16 @@
         <f t="shared" si="0"/>
         <v>writeSPI1(0x26);writeSPI1(SMARTRF_SETTING_FSCAL0);</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="K25" t="str">
+        <f t="shared" si="1"/>
+        <v>writeSPI1(SMARTRF_SETTING_FSCAL1);</v>
+      </c>
+      <c r="O25" t="str">
+        <f t="shared" si="2"/>
+        <v>writeSPI1(0x26);</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>44</v>
       </c>
@@ -1274,8 +1462,16 @@
         <f t="shared" si="0"/>
         <v>writeSPI1(0x29);writeSPI1(SMARTRF_SETTING_FSTEST);</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="K26" t="str">
+        <f t="shared" si="1"/>
+        <v>writeSPI1(0x29);</v>
+      </c>
+      <c r="O26" t="str">
+        <f t="shared" si="2"/>
+        <v>writeSPI1(SMARTRF_SETTING_FSCAL0);</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>46</v>
       </c>
@@ -1292,8 +1488,16 @@
         <f t="shared" si="0"/>
         <v>writeSPI1(0x2C);writeSPI1(SMARTRF_SETTING_TEST2);</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="K27" t="str">
+        <f t="shared" si="1"/>
+        <v>writeSPI1(SMARTRF_SETTING_FSTEST);</v>
+      </c>
+      <c r="O27" t="str">
+        <f t="shared" si="2"/>
+        <v>writeSPI1(0x2C);</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>48</v>
       </c>
@@ -1310,8 +1514,16 @@
         <f t="shared" si="0"/>
         <v>writeSPI1(0x2D);writeSPI1(SMARTRF_SETTING_TEST1);</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="K28" t="str">
+        <f t="shared" si="1"/>
+        <v>writeSPI1(0x2D);</v>
+      </c>
+      <c r="O28" t="str">
+        <f t="shared" si="2"/>
+        <v>writeSPI1(SMARTRF_SETTING_TEST2);</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>50</v>
       </c>
@@ -1328,8 +1540,16 @@
         <f t="shared" si="0"/>
         <v>writeSPI1(0x2E);writeSPI1(SMARTRF_SETTING_TEST0);</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="K29" t="str">
+        <f t="shared" si="1"/>
+        <v>writeSPI1(SMARTRF_SETTING_TEST1);</v>
+      </c>
+      <c r="O29" t="str">
+        <f t="shared" si="2"/>
+        <v>writeSPI1(0x2E);</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>52</v>
       </c>
@@ -1346,8 +1566,16 @@
         <f t="shared" si="0"/>
         <v>writeSPI1(0x03);writeSPI1(SMARTRF_SETTING_FIFOTHR);</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="K30" t="str">
+        <f t="shared" si="1"/>
+        <v>writeSPI1(0x03);</v>
+      </c>
+      <c r="O30" t="str">
+        <f t="shared" si="2"/>
+        <v>writeSPI1(SMARTRF_SETTING_TEST0);</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>54</v>
       </c>
@@ -1364,8 +1592,16 @@
         <f t="shared" si="0"/>
         <v>writeSPI1(0x00);writeSPI1(SMARTRF_SETTING_IOCFG2);</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="K31" t="str">
+        <f t="shared" si="1"/>
+        <v>writeSPI1(SMARTRF_SETTING_FIFOTHR);</v>
+      </c>
+      <c r="O31" t="str">
+        <f t="shared" si="2"/>
+        <v>writeSPI1(0x00);</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>56</v>
       </c>
@@ -1382,8 +1618,16 @@
         <f t="shared" si="0"/>
         <v>writeSPI1(0x02);writeSPI1(SMARTRF_SETTING_IOCFG0D);</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="K32" t="str">
+        <f t="shared" si="1"/>
+        <v>writeSPI1(0x02);</v>
+      </c>
+      <c r="O32" t="str">
+        <f t="shared" si="2"/>
+        <v>writeSPI1(SMARTRF_SETTING_IOCFG2);</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>57</v>
       </c>
@@ -1400,8 +1644,16 @@
         <f t="shared" si="0"/>
         <v>writeSPI1(0x07);writeSPI1(SMARTRF_SETTING_PKTCTRL1);</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="K33" t="str">
+        <f t="shared" si="1"/>
+        <v>writeSPI1(SMARTRF_SETTING_IOCFG0D);</v>
+      </c>
+      <c r="O33" t="str">
+        <f t="shared" si="2"/>
+        <v>writeSPI1(0x07);</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>59</v>
       </c>
@@ -1418,8 +1670,16 @@
         <f t="shared" si="0"/>
         <v>writeSPI1(0x08);writeSPI1(SMARTRF_SETTING_PKTCTRL0);</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="K34" t="str">
+        <f t="shared" si="1"/>
+        <v>writeSPI1(0x08);</v>
+      </c>
+      <c r="O34" t="str">
+        <f t="shared" si="2"/>
+        <v>writeSPI1(SMARTRF_SETTING_PKTCTRL1);</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>61</v>
       </c>
@@ -1436,8 +1696,16 @@
         <f t="shared" si="0"/>
         <v>writeSPI1(0x09);writeSPI1(SMARTRF_SETTING_ADDR);</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="K35" t="str">
+        <f t="shared" si="1"/>
+        <v>writeSPI1(SMARTRF_SETTING_PKTCTRL0);</v>
+      </c>
+      <c r="O35" t="str">
+        <f t="shared" si="2"/>
+        <v>writeSPI1(0x09);</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>62</v>
       </c>
@@ -1453,6 +1721,20 @@
       <c r="E36" t="str">
         <f t="shared" si="0"/>
         <v>writeSPI1(0x06);writeSPI1(SMARTRF_SETTING_PKTLEN);</v>
+      </c>
+      <c r="K36" t="str">
+        <f t="shared" si="1"/>
+        <v>writeSPI1(0x06);</v>
+      </c>
+      <c r="O36" t="str">
+        <f>IF(ISODD(ROW($K36)),"writeSPI1("&amp;$C36&amp;");","writeSPI1("&amp;$A35&amp;");")</f>
+        <v>writeSPI1(SMARTRF_SETTING_ADDR);</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="K37" t="str">
+        <f t="shared" si="1"/>
+        <v>writeSPI1(SMARTRF_SETTING_PKTLEN);</v>
       </c>
     </row>
   </sheetData>

</xml_diff>